<commit_message>
communiaction db -> crawler
</commit_message>
<xml_diff>
--- a/db/initial_data/initial_data.xlsx
+++ b/db/initial_data/initial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAN\Desktop\flixbus_project\db\initial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DB76D4-DADF-41E2-8322-AF749F93811D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E092FBD-7C34-4561-A1D2-84A1122D4190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="15375" windowHeight="7875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BC2A4C-487C-4EA0-9E71-294F11F9D7FE}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
         <v>1815</v>
       </c>
       <c r="E2" s="2">
-        <v>43811</v>
+        <v>43832</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>7588</v>
       </c>
       <c r="E3" s="2">
-        <v>43811</v>
+        <v>43832</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>7588</v>
       </c>
       <c r="E4" s="2">
-        <v>43812</v>
+        <v>43833</v>
       </c>
     </row>
   </sheetData>
@@ -763,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8384F5-AAB9-43F9-B53A-4731A3C10E78}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Stan aplikacji z logowaniem oraz autoryzacją, a także widokiem usera i admina
</commit_message>
<xml_diff>
--- a/db/initial_data/initial_data.xlsx
+++ b/db/initial_data/initial_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAN\Desktop\flixbus_project\db\initial_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Desktop\flixPytonek\flixbus_project\db\initial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E092FBD-7C34-4561-A1D2-84A1122D4190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB5F491-B680-483E-85CE-A6D6C7ADCFC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="915" windowWidth="18000" windowHeight="9360" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="requests" sheetId="3" r:id="rId3"/>
     <sheet name="distances" sheetId="4" r:id="rId4"/>
     <sheet name="cities" sheetId="6" r:id="rId5"/>
+    <sheet name="results" sheetId="7" r:id="rId6"/>
+    <sheet name="working_days" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>user_id</t>
   </si>
@@ -104,6 +106,63 @@
   </si>
   <si>
     <t>city_name</t>
+  </si>
+  <si>
+    <t>test2_job</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">price </t>
+  </si>
+  <si>
+    <t>changes_number</t>
+  </si>
+  <si>
+    <t>69.99</t>
+  </si>
+  <si>
+    <t>result_id</t>
+  </si>
+  <si>
+    <t>39.99</t>
+  </si>
+  <si>
+    <t>55.99</t>
+  </si>
+  <si>
+    <t>59.99</t>
+  </si>
+  <si>
+    <t>45.99</t>
+  </si>
+  <si>
+    <t>49.99</t>
+  </si>
+  <si>
+    <t>129.99</t>
+  </si>
+  <si>
+    <t>95.98</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>105.98</t>
+  </si>
+  <si>
+    <t>119.98</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>working</t>
   </si>
 </sst>
 </file>
@@ -139,10 +198,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -454,7 +514,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,10 +609,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9866DEF6-904D-43B5-A1D1-93F933E91EE9}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +657,23 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43749</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -604,10 +681,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BC2A4C-487C-4EA0-9E71-294F11F9D7FE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +721,7 @@
         <v>1915</v>
       </c>
       <c r="D2">
-        <v>1815</v>
+        <v>7588</v>
       </c>
       <c r="E2" s="2">
         <v>43832</v>
@@ -664,7 +741,7 @@
         <v>7588</v>
       </c>
       <c r="E3" s="2">
-        <v>43832</v>
+        <v>43833</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,7 +758,24 @@
         <v>7588</v>
       </c>
       <c r="E4" s="2">
-        <v>43833</v>
+        <v>43834</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1915</v>
+      </c>
+      <c r="D5">
+        <v>1815</v>
+      </c>
+      <c r="E5" s="2">
+        <v>43832</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +788,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8384F5-AAB9-43F9-B53A-4731A3C10E78}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -804,4 +898,1435 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CB85B4-8747-47D8-B796-58E3CE25854C}">
+  <dimension ref="A1:I59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1577728921</v>
+      </c>
+      <c r="D2">
+        <v>1915</v>
+      </c>
+      <c r="E2">
+        <v>7588</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1577728980</v>
+      </c>
+      <c r="D3">
+        <v>1915</v>
+      </c>
+      <c r="E3">
+        <v>7588</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G3" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1577729000</v>
+      </c>
+      <c r="D4">
+        <v>1915</v>
+      </c>
+      <c r="E4">
+        <v>7588</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1577729242</v>
+      </c>
+      <c r="D5">
+        <v>1915</v>
+      </c>
+      <c r="E5">
+        <v>7588</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="G5" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1577729540</v>
+      </c>
+      <c r="D6">
+        <v>1915</v>
+      </c>
+      <c r="E6">
+        <v>7588</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1577730200</v>
+      </c>
+      <c r="D7">
+        <v>1915</v>
+      </c>
+      <c r="E7">
+        <v>7588</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="G7" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1577730280</v>
+      </c>
+      <c r="D8">
+        <v>1915</v>
+      </c>
+      <c r="E8">
+        <v>7588</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1577730350</v>
+      </c>
+      <c r="D9">
+        <v>1915</v>
+      </c>
+      <c r="E9">
+        <v>7588</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G9" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1577730700</v>
+      </c>
+      <c r="D10">
+        <v>1915</v>
+      </c>
+      <c r="E10">
+        <v>7588</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1577730956</v>
+      </c>
+      <c r="D11">
+        <v>1915</v>
+      </c>
+      <c r="E11">
+        <v>7588</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="G11" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1577731201</v>
+      </c>
+      <c r="D12">
+        <v>1915</v>
+      </c>
+      <c r="E12">
+        <v>7588</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G12" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1577731400</v>
+      </c>
+      <c r="D13">
+        <v>1915</v>
+      </c>
+      <c r="E13">
+        <v>7588</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="G13" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>1577731470</v>
+      </c>
+      <c r="D14">
+        <v>1915</v>
+      </c>
+      <c r="E14">
+        <v>7588</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>1577731620</v>
+      </c>
+      <c r="D15">
+        <v>1915</v>
+      </c>
+      <c r="E15">
+        <v>7588</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G15" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>1577731840</v>
+      </c>
+      <c r="D16">
+        <v>1915</v>
+      </c>
+      <c r="E16">
+        <v>7588</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1577732100</v>
+      </c>
+      <c r="D17">
+        <v>1915</v>
+      </c>
+      <c r="E17">
+        <v>7588</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="G17" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>1577732200</v>
+      </c>
+      <c r="D18">
+        <v>1915</v>
+      </c>
+      <c r="E18">
+        <v>7588</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G18" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>1577732300</v>
+      </c>
+      <c r="D19">
+        <v>1915</v>
+      </c>
+      <c r="E19">
+        <v>7588</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="G19" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>1577732400</v>
+      </c>
+      <c r="D20">
+        <v>1915</v>
+      </c>
+      <c r="E20">
+        <v>1815</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G20" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1577732500</v>
+      </c>
+      <c r="D21">
+        <v>1915</v>
+      </c>
+      <c r="E21">
+        <v>1815</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="G21" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>1577732600</v>
+      </c>
+      <c r="D22">
+        <v>1915</v>
+      </c>
+      <c r="E22">
+        <v>1815</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>1577732700</v>
+      </c>
+      <c r="D23">
+        <v>1915</v>
+      </c>
+      <c r="E23">
+        <v>1815</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G23" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>1577732800</v>
+      </c>
+      <c r="D24">
+        <v>1915</v>
+      </c>
+      <c r="E24">
+        <v>1815</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="G24" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H24">
+        <v>128</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>1577732900</v>
+      </c>
+      <c r="D25">
+        <v>1915</v>
+      </c>
+      <c r="E25">
+        <v>1815</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="G25" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1577728921</v>
+      </c>
+      <c r="D36">
+        <v>1915</v>
+      </c>
+      <c r="E36">
+        <v>7588</v>
+      </c>
+      <c r="F36" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G36" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1577728980</v>
+      </c>
+      <c r="D37">
+        <v>1915</v>
+      </c>
+      <c r="E37">
+        <v>7588</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G37" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1577729000</v>
+      </c>
+      <c r="D38">
+        <v>1915</v>
+      </c>
+      <c r="E38">
+        <v>7588</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1577729242</v>
+      </c>
+      <c r="D39">
+        <v>1915</v>
+      </c>
+      <c r="E39">
+        <v>7588</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="G39" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1577729540</v>
+      </c>
+      <c r="D40">
+        <v>1915</v>
+      </c>
+      <c r="E40">
+        <v>7588</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G40" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1577730200</v>
+      </c>
+      <c r="D41">
+        <v>1915</v>
+      </c>
+      <c r="E41">
+        <v>7588</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="G41" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>1577730280</v>
+      </c>
+      <c r="D42">
+        <v>1915</v>
+      </c>
+      <c r="E42">
+        <v>7588</v>
+      </c>
+      <c r="F42" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G42" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>1577730350</v>
+      </c>
+      <c r="D43">
+        <v>1915</v>
+      </c>
+      <c r="E43">
+        <v>7588</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G43" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>1577730700</v>
+      </c>
+      <c r="D44">
+        <v>1915</v>
+      </c>
+      <c r="E44">
+        <v>7588</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>1577730956</v>
+      </c>
+      <c r="D45">
+        <v>1915</v>
+      </c>
+      <c r="E45">
+        <v>7588</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="G45" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>11</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>1577731201</v>
+      </c>
+      <c r="D46">
+        <v>1915</v>
+      </c>
+      <c r="E46">
+        <v>7588</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G46" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>1577731400</v>
+      </c>
+      <c r="D47">
+        <v>1915</v>
+      </c>
+      <c r="E47">
+        <v>7588</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="G47" s="2">
+        <v>43833</v>
+      </c>
+      <c r="H47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>13</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>1577731470</v>
+      </c>
+      <c r="D48">
+        <v>1915</v>
+      </c>
+      <c r="E48">
+        <v>7588</v>
+      </c>
+      <c r="F48" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G48" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>1577731620</v>
+      </c>
+      <c r="D49">
+        <v>1915</v>
+      </c>
+      <c r="E49">
+        <v>7588</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G49" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>1577731840</v>
+      </c>
+      <c r="D50">
+        <v>1915</v>
+      </c>
+      <c r="E50">
+        <v>7588</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G50" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>16</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>1577732100</v>
+      </c>
+      <c r="D51">
+        <v>1915</v>
+      </c>
+      <c r="E51">
+        <v>7588</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="G51" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>17</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>1577732200</v>
+      </c>
+      <c r="D52">
+        <v>1915</v>
+      </c>
+      <c r="E52">
+        <v>7588</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G52" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>1577732300</v>
+      </c>
+      <c r="D53">
+        <v>1915</v>
+      </c>
+      <c r="E53">
+        <v>7588</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="G53" s="2">
+        <v>43834</v>
+      </c>
+      <c r="H53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>1577732400</v>
+      </c>
+      <c r="D54">
+        <v>1915</v>
+      </c>
+      <c r="E54">
+        <v>1815</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="G54" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>1577732500</v>
+      </c>
+      <c r="D55">
+        <v>1915</v>
+      </c>
+      <c r="E55">
+        <v>1815</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="G55" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>1577732600</v>
+      </c>
+      <c r="D56">
+        <v>1915</v>
+      </c>
+      <c r="E56">
+        <v>1815</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G56" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>1577732700</v>
+      </c>
+      <c r="D57">
+        <v>1915</v>
+      </c>
+      <c r="E57">
+        <v>1815</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G57" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H57" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>1577732800</v>
+      </c>
+      <c r="D58">
+        <v>1915</v>
+      </c>
+      <c r="E58">
+        <v>1815</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="G58" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H58">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>1577732900</v>
+      </c>
+      <c r="D59">
+        <v>1915</v>
+      </c>
+      <c r="E59">
+        <v>1815</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="G59" s="2">
+        <v>43832</v>
+      </c>
+      <c r="H59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6FDD4-552A-4501-B8F2-3DE81D9ECC08}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43832</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>43833</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>43834</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>